<commit_message>
good count for popularity => need refactor
</commit_message>
<xml_diff>
--- a/RS-OP-2016/result_graphs.xlsx
+++ b/RS-OP-2016/result_graphs.xlsx
@@ -235,37 +235,37 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="11"/>
                 <c:pt idx="0">
-                  <c:v>-0.031</c:v>
+                  <c:v>-0.1</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>-0.029</c:v>
+                  <c:v>-0.076</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>-0.014</c:v>
+                  <c:v>-0.049</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.006</c:v>
+                  <c:v>-0.022</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.044</c:v>
+                  <c:v>0.023</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.12</c:v>
+                  <c:v>0.095</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.248</c:v>
+                  <c:v>0.244</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.395</c:v>
+                  <c:v>0.441</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.594</c:v>
+                  <c:v>0.626</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.704</c:v>
+                  <c:v>0.711</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0.749</c:v>
+                  <c:v>0.748</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -371,37 +371,37 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="11"/>
                 <c:pt idx="0">
-                  <c:v>0.756</c:v>
+                  <c:v>0.751</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.756</c:v>
+                  <c:v>0.75</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.755</c:v>
+                  <c:v>0.749</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.754</c:v>
+                  <c:v>0.746</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.746</c:v>
+                  <c:v>0.74</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.732</c:v>
+                  <c:v>0.726</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.694</c:v>
+                  <c:v>0.684</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.63</c:v>
+                  <c:v>0.61</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.538</c:v>
+                  <c:v>0.526</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.466</c:v>
+                  <c:v>0.469</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0.399</c:v>
+                  <c:v>0.415</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1542,7 +1542,7 @@
   <dimension ref="A1:C14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1573,10 +1573,10 @@
         <v>0</v>
       </c>
       <c r="B4">
-        <v>-3.1E-2</v>
+        <v>-0.1</v>
       </c>
       <c r="C4">
-        <v>0.75600000000000001</v>
+        <v>0.751</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
@@ -1584,10 +1584,10 @@
         <v>0.1</v>
       </c>
       <c r="B5">
-        <v>-2.9000000000000001E-2</v>
+        <v>-7.5999999999999998E-2</v>
       </c>
       <c r="C5">
-        <v>0.75600000000000001</v>
+        <v>0.75</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
@@ -1595,10 +1595,10 @@
         <v>0.2</v>
       </c>
       <c r="B6">
-        <v>-1.4E-2</v>
+        <v>-4.9000000000000002E-2</v>
       </c>
       <c r="C6">
-        <v>0.755</v>
+        <v>0.749</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
@@ -1606,10 +1606,10 @@
         <v>0.3</v>
       </c>
       <c r="B7">
-        <v>6.0000000000000001E-3</v>
+        <v>-2.1999999999999999E-2</v>
       </c>
       <c r="C7">
-        <v>0.754</v>
+        <v>0.746</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
@@ -1617,10 +1617,10 @@
         <v>0.4</v>
       </c>
       <c r="B8">
-        <v>4.3999999999999997E-2</v>
+        <v>2.3E-2</v>
       </c>
       <c r="C8">
-        <v>0.746</v>
+        <v>0.74</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
@@ -1628,10 +1628,10 @@
         <v>0.5</v>
       </c>
       <c r="B9">
-        <v>0.12</v>
+        <v>9.5000000000000001E-2</v>
       </c>
       <c r="C9">
-        <v>0.73199999999999998</v>
+        <v>0.72599999999999998</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
@@ -1639,10 +1639,10 @@
         <v>0.6</v>
       </c>
       <c r="B10">
-        <v>0.248</v>
+        <v>0.24399999999999999</v>
       </c>
       <c r="C10">
-        <v>0.69399999999999995</v>
+        <v>0.68400000000000005</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.2">
@@ -1650,10 +1650,10 @@
         <v>0.7</v>
       </c>
       <c r="B11">
-        <v>0.39500000000000002</v>
+        <v>0.441</v>
       </c>
       <c r="C11">
-        <v>0.63</v>
+        <v>0.61</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.2">
@@ -1661,10 +1661,10 @@
         <v>0.8</v>
       </c>
       <c r="B12">
-        <v>0.59399999999999997</v>
+        <v>0.626</v>
       </c>
       <c r="C12">
-        <v>0.53800000000000003</v>
+        <v>0.52600000000000002</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.2">
@@ -1672,10 +1672,10 @@
         <v>0.9</v>
       </c>
       <c r="B13">
-        <v>0.70399999999999996</v>
+        <v>0.71099999999999997</v>
       </c>
       <c r="C13">
-        <v>0.46600000000000003</v>
+        <v>0.46899999999999997</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.2">
@@ -1683,10 +1683,10 @@
         <v>1</v>
       </c>
       <c r="B14">
-        <v>0.749</v>
+        <v>0.748</v>
       </c>
       <c r="C14">
-        <v>0.39900000000000002</v>
+        <v>0.41499999999999998</v>
       </c>
     </row>
   </sheetData>

</xml_diff>